<commit_message>
Created Dice and rolling
</commit_message>
<xml_diff>
--- a/Reference/Marks.xlsx
+++ b/Reference/Marks.xlsx
@@ -23,10 +23,113 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Internal Docs</t>
+  </si>
+  <si>
+    <t>Sound on click</t>
+  </si>
+  <si>
+    <t>Dice roll animation</t>
+  </si>
+  <si>
+    <t>Background image of board</t>
+  </si>
+  <si>
+    <t>Bonus 1</t>
+  </si>
+  <si>
+    <t>Bonus 2</t>
+  </si>
+  <si>
+    <t>Bonus 3</t>
+  </si>
+  <si>
+    <t>Bonus 4</t>
+  </si>
+  <si>
+    <t>Buttons to navigate between scenes</t>
+  </si>
+  <si>
+    <t>Another scene for project with 4d6</t>
+  </si>
+  <si>
+    <t>Result label shows tally</t>
+  </si>
+  <si>
+    <t>Drop lowest value from result</t>
+  </si>
+  <si>
+    <t>Start from template</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Roll button</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Random 2d6</t>
+  </si>
+  <si>
+    <t>Display result using images</t>
+  </si>
+  <si>
+    <t>Text label for result</t>
+  </si>
+  <si>
+    <t>Program header: Source file, author, date, description</t>
+  </si>
+  <si>
+    <t>Header for all functions</t>
+  </si>
+  <si>
+    <t>Contextual var names</t>
+  </si>
+  <si>
+    <t>Version Control</t>
+  </si>
+  <si>
+    <t>Repo contains code and is well-structured</t>
+  </si>
+  <si>
+    <t>Include commits that show work progress</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,8 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +442,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3">
+        <f>8/4</f>
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" ref="C21:C23" si="0">8/4</f>
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added labels, added dice to 4d6
</commit_message>
<xml_diff>
--- a/Reference/Marks.xlsx
+++ b/Reference/Marks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Category</t>
   </si>
@@ -446,7 +446,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +509,9 @@
       <c r="C4" s="3">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -520,6 +523,9 @@
       <c r="C5" s="3">
         <v>2</v>
       </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -531,6 +537,9 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -578,6 +587,9 @@
       <c r="C11" s="3">
         <v>1</v>
       </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -642,6 +654,9 @@
       <c r="C18" s="3">
         <v>2</v>
       </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -652,6 +667,9 @@
       </c>
       <c r="C19" s="3">
         <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added background, added d46 calculation
</commit_message>
<xml_diff>
--- a/Reference/Marks.xlsx
+++ b/Reference/Marks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Category</t>
   </si>
@@ -446,7 +446,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +551,9 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -562,6 +565,9 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -713,6 +719,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -724,6 +733,9 @@
       <c r="C23" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>